<commit_message>
receive excel with to two columns to make easier the program
</commit_message>
<xml_diff>
--- a/juan/prueba.xlsx
+++ b/juan/prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eafit-my.sharepoint.com/personal/jjpiconc_eafit_edu_co/Documents/COSAS DE JUANJO/INTERNSHIP_2023_Oregon/COMPUTATIONAL/jaratest/juan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjpc/Documents/jaratest/juan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_598E0372172C44F0943FDFEF9D80A6B6638EB21A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13949C4E-9F75-7446-8514-FCF482A8F943}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5163C1-DB51-304E-9071-0970A53AB8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5480" yWindow="4000" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>IDs</t>
   </si>
   <si>
-    <t>Dates</t>
+    <t>RangeDates</t>
   </si>
   <si>
-    <t>[(2023-05-12, 2023-6-16),2023-6-17]</t>
+    <t>AloneDate</t>
+  </si>
+  <si>
+    <t>2023-6-17,2023-6-18</t>
+  </si>
+  <si>
+    <t>(2023-05-12, 2023-6-16), (2023-07-1, 2023-7-3)</t>
   </si>
 </sst>
 </file>
@@ -383,28 +389,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug with the alpha fixed. now I will change the tools to plot several plots for one mice and a range of dates
</commit_message>
<xml_diff>
--- a/juan/prueba.xlsx
+++ b/juan/prueba.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t xml:space="preserve">IDs</t>
   </si>
@@ -132,10 +132,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -160,6 +160,14 @@
       </c>
       <c r="C2" s="1"/>
     </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>